<commit_message>
Adding new functions, to incorporate combinations of parameters and bounds
</commit_message>
<xml_diff>
--- a/Excel_Results/YX_C pH_UL YX_N Xmax.xlsx
+++ b/Excel_Results/YX_C pH_UL YX_N Xmax.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK3"/>
+  <dimension ref="A1:BK6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,182 +441,312 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>YX_C_value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>YX_N_value</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Xmax_value</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>mu_max_value</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>pH_UL_value</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>RMSE_X_og</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_X_og</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>MAPE_X_og</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>RMSE_C_og</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_C_og</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>MAPE_C_og</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>RMSE_N_og</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_N_og</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>MAPE_N_og</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>RMSE_pH_og</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_pH_og</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>MAPE_pH_og</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>AIC_og</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>BIC_og</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>RMSE_og</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_og</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>MAPE_og</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>k_C_value</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>k_N_value</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>k_O_value</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>k_d_value</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>YX_CO2_value</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>YX_O2_value</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>pH_LL_value</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>I_val_value</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>O2_sat_value</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>RMSE_X_new</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_X_new</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>MAPE_X_new</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>RMSE_C_new</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_C_new</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>MAPE_C_new</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>RMSE_N_new</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_N_new</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>MAPE_N_new</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>RMSE_pH_new</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_pH_new</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>MAPE_pH_new</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>AIC_new</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>BIC_new</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>RMSE_new</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>NMRSE_new</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>MAPE_new</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_k_C</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_k_N</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_k_O</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_k_d</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_YX_CO2</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_YX_O2</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_YX_C</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_YX_N</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_Xmax</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_mu_max</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_pH_LL</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>t_value_pH_UL</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_I_val</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>t_value_O2_sat</t>
         </is>
       </c>
     </row>
@@ -627,63 +757,71 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>0.484</v>
+      </c>
+      <c r="C2" t="n">
+        <v>21.575</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.4462</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="F2" t="n">
         <v>7.4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.2005851692302318</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.2044719770418198</v>
-      </c>
-      <c r="E2" t="n">
-        <v>17.90493789151974</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.3615215812803811</v>
-      </c>
       <c r="G2" t="n">
-        <v>0.1586688041433045</v>
+        <v>0.2005372981607208</v>
       </c>
       <c r="H2" t="n">
-        <v>6.02365418992219</v>
+        <v>0.2044231783581305</v>
       </c>
       <c r="I2" t="n">
-        <v>0.06423696915458403</v>
+        <v>17.89660959514114</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5063994213229439</v>
+        <v>0.3567690347607395</v>
       </c>
       <c r="K2" t="n">
-        <v>6.51281349533272</v>
+        <v>0.1565829511487578</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1260098929727701</v>
+        <v>6.275208824109844</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1595061936364179</v>
+        <v>0.06388643378451481</v>
       </c>
       <c r="N2" t="n">
-        <v>1.44764375959904</v>
+        <v>0.5036360451722244</v>
       </c>
       <c r="O2" t="n">
-        <v>-109.5157925655658</v>
+        <v>6.472610915178476</v>
       </c>
       <c r="P2" t="n">
-        <v>-109.5157925655658</v>
+        <v>0.1260190425499805</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.2184817756586141</v>
+        <v>0.1595177753797221</v>
       </c>
       <c r="R2" t="n">
-        <v>0.03138961952683599</v>
+        <v>1.44759408904611</v>
       </c>
       <c r="S2" t="n">
-        <v>7.972262334093423</v>
-      </c>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
+        <v>-110.1771168589593</v>
+      </c>
+      <c r="T2" t="n">
+        <v>-110.1771168589593</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.2164841955112593</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.0311026240526789</v>
+      </c>
+      <c r="W2" t="n">
+        <v>8.023005855868893</v>
+      </c>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr"/>
@@ -698,6 +836,32 @@
       <c r="AI2" t="inlineStr"/>
       <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr"/>
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr"/>
+      <c r="AY2" t="inlineStr"/>
+      <c r="AZ2" t="inlineStr"/>
+      <c r="BA2" t="inlineStr"/>
+      <c r="BB2" t="inlineStr"/>
+      <c r="BC2" t="inlineStr"/>
+      <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="inlineStr"/>
+      <c r="BF2" t="inlineStr"/>
+      <c r="BG2" t="inlineStr"/>
+      <c r="BH2" t="inlineStr"/>
+      <c r="BI2" t="inlineStr"/>
+      <c r="BJ2" t="inlineStr"/>
+      <c r="BK2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -706,12 +870,20 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.067612755409654</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+        <v>0.5014098088000311</v>
+      </c>
+      <c r="C3" t="n">
+        <v>7.978315519469787</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.199866067506358</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.07415454346322746</v>
+      </c>
+      <c r="F3" t="n">
+        <v>7.999775887261329</v>
+      </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -725,60 +897,463 @@
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
-      <c r="T3" t="n">
-        <v>15.8631917370161</v>
-      </c>
-      <c r="U3" t="n">
-        <v>16.17057825914417</v>
-      </c>
-      <c r="V3" t="n">
-        <v>1426.847686602278</v>
-      </c>
-      <c r="W3" t="n">
-        <v>33.03677465650261</v>
-      </c>
-      <c r="X3" t="n">
-        <v>14.49956461502002</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>693.0835178608298</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>0.680222192373185</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>5.362396905119608</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>62.7297039075708</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>1.18671094294346</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>1.502165750561341</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>16.95462265586217</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>211.4411800112042</v>
-      </c>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="n">
-        <v>213.0246989496603</v>
+        <v>0.1853035343914761</v>
       </c>
       <c r="AH3" t="n">
-        <v>18.33671397008586</v>
+        <v>0.1888942247089689</v>
       </c>
       <c r="AI3" t="n">
-        <v>2.634464468069787</v>
+        <v>14.13364015217479</v>
       </c>
       <c r="AJ3" t="n">
-        <v>549.9038827566351</v>
+        <v>0.45339292312622</v>
       </c>
       <c r="AK3" t="n">
-        <v>2922.910721411978</v>
-      </c>
+        <v>0.1989903691632765</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>8.245615372806443</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0.03448950833537922</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0.2718912067709616</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>2.983676993903245</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0.15424975329665</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0.1952528522742405</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>1.62741351764715</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>-87.73113184158903</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>-79.81353714930849</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0.2573349253289403</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>0.03697171250413035</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>6.747586509132905</v>
+      </c>
+      <c r="AX3" t="inlineStr"/>
+      <c r="AY3" t="inlineStr"/>
+      <c r="AZ3" t="inlineStr"/>
+      <c r="BA3" t="inlineStr"/>
+      <c r="BB3" t="inlineStr"/>
+      <c r="BC3" t="inlineStr"/>
+      <c r="BD3" t="n">
+        <v>12.79815873672886</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>22323.50740259796</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>40297.26392915168</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>315.528626489602</v>
+      </c>
+      <c r="BH3" t="inlineStr"/>
+      <c r="BI3" t="n">
+        <v>167.4981950610008</v>
+      </c>
+      <c r="BJ3" t="inlineStr"/>
+      <c r="BK3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Model3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.4999985119978698</v>
+      </c>
+      <c r="C4" t="n">
+        <v>7.999878057301657</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.199998890836386</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.08220624099804874</v>
+      </c>
+      <c r="F4" t="n">
+        <v>7.90714109502078</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="n">
+        <v>0.1848992429216794</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0.1884820991443137</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>14.18983274596963</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0.4516141993229766</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>0.1982097021343199</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>8.222597135366303</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0.03460301886020422</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>0.2727860445075789</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>3.013473960890303</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>0.1537951290646534</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0.1946773785628524</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>1.62904589866373</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>-87.98914180051263</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>-80.07154710823208</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>0.2564144232007028</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>0.03683946251901413</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>6.763737435222493</v>
+      </c>
+      <c r="AX4" t="inlineStr"/>
+      <c r="AY4" t="inlineStr"/>
+      <c r="AZ4" t="inlineStr"/>
+      <c r="BA4" t="inlineStr"/>
+      <c r="BB4" t="inlineStr"/>
+      <c r="BC4" t="inlineStr"/>
+      <c r="BD4" t="n">
+        <v>12.79564733694141</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>21958.61103834778</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>39573.19893004595</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>341.3633301330285</v>
+      </c>
+      <c r="BH4" t="inlineStr"/>
+      <c r="BI4" t="n">
+        <v>162.7766670853489</v>
+      </c>
+      <c r="BJ4" t="inlineStr"/>
+      <c r="BK4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Model4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5003809137327545</v>
+      </c>
+      <c r="C5" t="n">
+        <v>7.999994437168722</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.19999988156905</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.07835770453482455</v>
+      </c>
+      <c r="F5" t="n">
+        <v>7.949047067464349</v>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="n">
+        <v>0.1855311452603239</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0.1891262460719047</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>14.22284292980032</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0.4531914137063554</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>0.198901928361042</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>8.248370859536285</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>0.03465975885385188</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>0.2732333430076045</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>3.016296918873625</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>0.1543147095302978</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>0.1953350753548073</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>1.633390852881998</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>-87.74016588275413</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>-79.82257119047358</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.2573026388224573</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>0.03696707385108346</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>6.780225390273056</v>
+      </c>
+      <c r="AX5" t="inlineStr"/>
+      <c r="AY5" t="inlineStr"/>
+      <c r="AZ5" t="inlineStr"/>
+      <c r="BA5" t="inlineStr"/>
+      <c r="BB5" t="inlineStr"/>
+      <c r="BC5" t="inlineStr"/>
+      <c r="BD5" t="n">
+        <v>12.99654519725406</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>23682.68323268519</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>40317.52009190606</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>331.2842631397151</v>
+      </c>
+      <c r="BH5" t="inlineStr"/>
+      <c r="BI5" t="n">
+        <v>175.4103299371563</v>
+      </c>
+      <c r="BJ5" t="inlineStr"/>
+      <c r="BK5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Model5</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4990065055658796</v>
+      </c>
+      <c r="C6" t="n">
+        <v>7.998863246668955</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.199918296972637</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.07383212704294397</v>
+      </c>
+      <c r="F6" t="n">
+        <v>7.999999880767825</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="n">
+        <v>0.1865949809761084</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0.1902106960982398</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>14.31041591208651</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0.4531117951866366</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>0.1988669844573705</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>8.213820395628394</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.03476951804282848</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0.274098607831181</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>3.025442215489301</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>0.155141618185945</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0.1963817951720823</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>1.642383134341922</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>-87.66042427262151</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>-79.74282958034097</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.257587765111726</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.03700803839245201</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>6.798015414386533</v>
+      </c>
+      <c r="AX6" t="inlineStr"/>
+      <c r="AY6" t="inlineStr"/>
+      <c r="AZ6" t="inlineStr"/>
+      <c r="BA6" t="inlineStr"/>
+      <c r="BB6" t="inlineStr"/>
+      <c r="BC6" t="inlineStr"/>
+      <c r="BD6" t="n">
+        <v>12.8279616912902</v>
+      </c>
+      <c r="BE6" t="n">
+        <v>21812.86319368141</v>
+      </c>
+      <c r="BF6" t="n">
+        <v>40366.95696163853</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>311.7842338542818</v>
+      </c>
+      <c r="BH6" t="inlineStr"/>
+      <c r="BI6" t="n">
+        <v>163.9455856078934</v>
+      </c>
+      <c r="BJ6" t="inlineStr"/>
+      <c r="BK6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>